<commit_message>
Predictive Score is coming
</commit_message>
<xml_diff>
--- a/Predictive Score Doc/Xlsx/PGName.xlsx
+++ b/Predictive Score Doc/Xlsx/PGName.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Predictive Score\Doc\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Predictive-Score\Predictive Score Doc\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086836CF-AA07-4943-9962-EA7A54B75C0B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983EF993-8B52-4483-AA5D-CC649653B832}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{DE847C9C-91A3-4026-9DD0-59B63D3C3CCC}"/>
   </bookViews>

</xml_diff>